<commit_message>
Actualiza el historial de clientes con nuevos datos y corrige la fecha de última modificación. Añade manejo específico para un modal opcional antes de la descarga del PDF en la página de Fasecolda.
</commit_message>
<xml_diff>
--- a/Bases Consolidados/PANTILLA FODELSA N.xlsx
+++ b/Bases Consolidados/PANTILLA FODELSA N.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\PROYECTOS\AGENCIA INFONDO\COTIZACIONES\MCP\Bases Consolidados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AD667E-FBCB-49C2-8713-4EE2977E2C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136A42E8-4F4E-4753-8ED2-0E0D2CC79AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4DEF1856-761C-4FC4-A841-9B5775C87BF6}"/>
   </bookViews>
@@ -317,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -342,18 +342,21 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -363,19 +366,13 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -801,184 +798,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8971C112-9AF6-42D6-81AB-E2C154B579CA}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="43.42578125" customWidth="1"/>
     <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="59.1" customHeight="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:3" ht="59.1" customHeight="1">
+      <c r="A1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="23"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="14" t="s">
+      <c r="B1" s="21"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="16"/>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="14" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="17"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="15" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="16"/>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="14" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17"/>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="17"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="15" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="16"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="14" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="17"/>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="15" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="16"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="14" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="17"/>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="4"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="17"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="15" t="s">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="16"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="14" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="17"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="15" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="16"/>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+    </row>
+    <row r="18" spans="1:3">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="18" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="18"/>
+    <row r="20" spans="1:3">
+      <c r="A20" s="19"/>
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:3">
       <c r="A21" s="5"/>
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:3">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:3">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="18" t="s">
+    <row r="25" spans="1:3">
+      <c r="A25" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="18"/>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="B25" s="19"/>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="5"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:3">
       <c r="A27" s="5"/>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" ht="15.75">
-      <c r="A29" s="19" t="s">
+    <row r="29" spans="1:3" ht="15.75">
+      <c r="A29" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="19"/>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="B29" s="16"/>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="5"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" ht="15.75">
-      <c r="A32" s="19" t="s">
+    <row r="32" spans="1:3" ht="15.75">
+      <c r="A32" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="16"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="5" t="s">
@@ -1008,29 +1020,29 @@
       <c r="A36" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="12"/>
+      <c r="B36" s="22"/>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="13"/>
+      <c r="B37" s="10"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="21"/>
+      <c r="B39" s="15"/>
     </row>
     <row r="40" spans="1:2" ht="44.25" customHeight="1">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="20"/>
+      <c r="B40" s="14"/>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1"/>
@@ -1069,14 +1081,28 @@
       <c r="B49" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="21">
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1091,15 +1117,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A46240E9C16ACF4580208BCDD1584C19" ma:contentTypeVersion="1" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c123b30116eb1696ed6760edbcdae06c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cb24288e-bf72-47ae-a461-19b0293297a2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a9259aa4610e07bbb8461321e94cbc80" ns3:_="">
     <xsd:import namespace="cb24288e-bf72-47ae-a461-19b0293297a2"/>
@@ -1225,6 +1242,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059BE399-E90A-4F5C-8B54-187AC91B948A}">
   <ds:schemaRefs>
@@ -1242,14 +1268,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98AAA9BD-141C-449E-9A5F-E23FE59D0BF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F720539-AD5F-4FC3-9414-E2EE1548D97C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1265,4 +1283,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98AAA9BD-141C-449E-9A5F-E23FE59D0BF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Actualiza la plantilla de Excel y el historial de clientes. Cambia nombres de fondos, corrige fechas y valores asegurados, y mejora el manejo de fechas de vigencia y cálculo de días de cobertura en el manejador de plantillas.
</commit_message>
<xml_diff>
--- a/Bases Consolidados/PANTILLA FODELSA N.xlsx
+++ b/Bases Consolidados/PANTILLA FODELSA N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\PROYECTOS\AGENCIA INFONDO\COTIZACIONES\MCP\Bases Consolidados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136A42E8-4F4E-4753-8ED2-0E0D2CC79AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AB47EB-75B6-49E0-8A81-93696861E0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4DEF1856-761C-4FC4-A841-9B5775C87BF6}"/>
+    <workbookView xWindow="11985" yWindow="4365" windowWidth="19200" windowHeight="11175" xr2:uid="{4DEF1856-761C-4FC4-A841-9B5775C87BF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Autos" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Fecha De Cotización</t>
   </si>
@@ -92,9 +92,6 @@
     <t>La presente cotización no constituye aceptación del riesgo por parte de LAS COMPAÑIAS ASEGURADORAS, hasta tanto la compañía se manifieste de manera expresa y en documento escrito. Este documento es una cotización de SEGUROS de su vehículo; en caso de expedirse la póliza las condiciones de esta oferta pueden variar. Los términos de la cotización están sujetos a las condiciones generales y particulares del seguro que se cotiza, así como cambios en la medida en que se modifique la legislación tributaria. Esta cotización tiene una vigencia de 15 días calendario posteriores a su elaboración.</t>
   </si>
   <si>
-    <t>LINEAS DE ASISTENCIA</t>
-  </si>
-  <si>
     <t>DEDUCIBLES</t>
   </si>
   <si>
@@ -117,13 +114,106 @@
   </si>
   <si>
     <t>COTIZACIÓN PÓLIZA COLECTIVA DE AUTOS FODELSA</t>
+  </si>
+  <si>
+    <t>Responsabilidad civil extracontractual</t>
+  </si>
+  <si>
+    <t>Daños a bienes de terceros</t>
+  </si>
+  <si>
+    <t>Muerte o lesión a una persona  o más personas</t>
+  </si>
+  <si>
+    <t>Asistencia jurídica en proceso penal y civil</t>
+  </si>
+  <si>
+    <t>Pérdida total por daños</t>
+  </si>
+  <si>
+    <t>Pérdida parcial por daños</t>
+  </si>
+  <si>
+    <t>Pérdida total por hurto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terremoto </t>
+  </si>
+  <si>
+    <t>Amparo patrimonial</t>
+  </si>
+  <si>
+    <t>Gastos de transporte por pérdida total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehículo de reemplazo por pérdida total </t>
+  </si>
+  <si>
+    <t>Vehículo de reemplazo por pérdida parcial</t>
+  </si>
+  <si>
+    <t>Asistencias</t>
+  </si>
+  <si>
+    <t>Accidentes personales al conductor</t>
+  </si>
+  <si>
+    <t>Reembolso de gastos exequiales</t>
+  </si>
+  <si>
+    <t>Incluida</t>
+  </si>
+  <si>
+    <t>Incluido</t>
+  </si>
+  <si>
+    <t>30.000 diarios hasta 30 días</t>
+  </si>
+  <si>
+    <t>Hasta por 30 días</t>
+  </si>
+  <si>
+    <t>Hasta por 7 días</t>
+  </si>
+  <si>
+    <t>Pérdida total hurto</t>
+  </si>
+  <si>
+    <t>Pérdida parcial hurto</t>
+  </si>
+  <si>
+    <t>Terremoto / AMIT</t>
+  </si>
+  <si>
+    <t>Sin deducible</t>
+  </si>
+  <si>
+    <t>1 SMMLV</t>
+  </si>
+  <si>
+    <t>10% - 1 SMMLV</t>
+  </si>
+  <si>
+    <t>SERVICIOS DE LA ASISTENCIA EN VIAJE</t>
+  </si>
+  <si>
+    <t>10 eventos por vigencia</t>
+  </si>
+  <si>
+    <t>Conductor elegido</t>
+  </si>
+  <si>
+    <t>Servicio de grúa</t>
+  </si>
+  <si>
+    <t>VALOR ASEGURADO AUTO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,8 +264,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial Rounded MT Bold"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,8 +326,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -271,26 +373,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -317,36 +399,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -354,25 +467,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -390,115 +488,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>89647</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>235586</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1109382</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>499565</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4C7CB8F-7C0F-4666-8C82-3DC9BB48EC6D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="89647" y="235586"/>
-          <a:ext cx="1019735" cy="263979"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2409264</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>235323</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3350558</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>594516</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CE191B0-5F5A-F39F-19C7-5B8F3F21749A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5300382" y="235323"/>
-          <a:ext cx="941294" cy="359193"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -798,325 +787,484 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8971C112-9AF6-42D6-81AB-E2C154B579CA}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="1" max="1" width="59.85546875" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="59.1" customHeight="1">
-      <c r="A1" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="21"/>
+      <c r="A1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="4"/>
+      <c r="A13" s="3"/>
       <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
     </row>
     <row r="18" spans="1:3">
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>25</v>
+      <c r="B19" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="19"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="10">
+        <v>1000000000</v>
+      </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="3"/>
+      <c r="A22" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="10">
+        <v>1000000000</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="3"/>
+      <c r="A23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="10">
+        <v>2000000000</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+      <c r="A24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="19"/>
+      <c r="A25" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="3"/>
+      <c r="A26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="3"/>
+      <c r="A27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.75">
-      <c r="A29" s="16" t="s">
+      <c r="A28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="13">
+        <v>30000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="16"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.75">
-      <c r="A32" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="16"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="9">
-        <v>45913</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="9">
-        <v>45974</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="10">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="22"/>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="10"/>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="1"/>
+      <c r="B38" s="21"/>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="15"/>
-    </row>
-    <row r="40" spans="1:2" ht="44.25" customHeight="1">
-      <c r="A40" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="14"/>
+      <c r="A39" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
+      <c r="A41" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
+      <c r="A42" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
+      <c r="A43" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
+      <c r="A44" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
+    <row r="46" spans="1:2" ht="15.75">
+      <c r="A46" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="22"/>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
+      <c r="A47" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
+      <c r="A48" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:2" ht="15.75">
+      <c r="A50" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="22"/>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="15"/>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="15">
+        <v>46029</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" s="16"/>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="17"/>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="18"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="2"/>
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="24"/>
+    </row>
+    <row r="58" spans="1:2" ht="71.099999999999994" customHeight="1">
+      <c r="A58" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="23"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A50:B50"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A32:B32"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A46240E9C16ACF4580208BCDD1584C19" ma:contentTypeVersion="1" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c123b30116eb1696ed6760edbcdae06c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cb24288e-bf72-47ae-a461-19b0293297a2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a9259aa4610e07bbb8461321e94cbc80" ns3:_="">
     <xsd:import namespace="cb24288e-bf72-47ae-a461-19b0293297a2"/>
@@ -1242,7 +1390,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1251,23 +1399,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059BE399-E90A-4F5C-8B54-187AC91B948A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="cb24288e-bf72-47ae-a461-19b0293297a2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F720539-AD5F-4FC3-9414-E2EE1548D97C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1285,10 +1423,26 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98AAA9BD-141C-449E-9A5F-E23FE59D0BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059BE399-E90A-4F5C-8B54-187AC91B948A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="cb24288e-bf72-47ae-a461-19b0293297a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>